<commit_message>
Add 2023 SDS items
</commit_message>
<xml_diff>
--- a/data-raw/Case closure item to name.xlsx
+++ b/data-raw/Case closure item to name.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbjanis/Box/CCMH/Data Repository/Data documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbjanis/Documents/Professional/CCMH R packages/CCMHr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A37E167-E39B-A74A-9AC6-0A08DA4E32C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E730FDAB-D5ED-5948-A455-21037F39CC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{577096A3-070E-624A-A6EF-FB0688A6F32A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15540" xr2:uid="{577096A3-070E-624A-A6EF-FB0688A6F32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Item</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>CLOSURE_04_108</t>
+  </si>
+  <si>
+    <t>Provided supportive documentation to campus partner (e.g. letter to professor, disability services)</t>
   </si>
 </sst>
 </file>
@@ -281,7 +287,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -300,9 +306,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -340,7 +346,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -446,7 +452,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -588,7 +594,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -596,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D699F59-D6A4-564D-A492-2D1231AE00D8}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,7 +642,7 @@
       <c r="B3">
         <v>102</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -647,7 +653,7 @@
       <c r="B4">
         <v>103</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -658,7 +664,7 @@
       <c r="B5">
         <v>104</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -669,7 +675,7 @@
       <c r="B6">
         <v>105</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -680,7 +686,7 @@
       <c r="B7">
         <v>106</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -691,7 +697,7 @@
       <c r="B8">
         <v>201</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -702,7 +708,7 @@
       <c r="B9">
         <v>202</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -713,7 +719,7 @@
       <c r="B10">
         <v>203</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>45</v>
       </c>
     </row>
@@ -724,7 +730,7 @@
       <c r="B11">
         <v>204</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>46</v>
       </c>
     </row>
@@ -735,7 +741,7 @@
       <c r="B12">
         <v>205</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>47</v>
       </c>
     </row>
@@ -746,7 +752,7 @@
       <c r="B13">
         <v>206</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>48</v>
       </c>
     </row>
@@ -757,7 +763,7 @@
       <c r="B14">
         <v>207</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -768,7 +774,7 @@
       <c r="B15">
         <v>208</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>71</v>
       </c>
     </row>
@@ -779,7 +785,7 @@
       <c r="B16">
         <v>209</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>50</v>
       </c>
     </row>
@@ -790,7 +796,7 @@
       <c r="B17">
         <v>301</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>51</v>
       </c>
     </row>
@@ -801,7 +807,7 @@
       <c r="B18">
         <v>302</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -812,7 +818,7 @@
       <c r="B19">
         <v>303</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>53</v>
       </c>
     </row>
@@ -823,7 +829,7 @@
       <c r="B20">
         <v>304</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>54</v>
       </c>
     </row>
@@ -834,7 +840,7 @@
       <c r="B21">
         <v>401</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>55</v>
       </c>
     </row>
@@ -842,7 +848,7 @@
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>56</v>
       </c>
     </row>
@@ -850,7 +856,7 @@
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>57</v>
       </c>
     </row>
@@ -858,7 +864,7 @@
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>58</v>
       </c>
     </row>
@@ -866,7 +872,7 @@
       <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>59</v>
       </c>
     </row>
@@ -874,7 +880,7 @@
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>60</v>
       </c>
     </row>
@@ -882,79 +888,87 @@
       <c r="A27" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>68</v>
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>69</v>
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>70</v>
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>62</v>
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>63</v>
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>64</v>
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>65</v>
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>